<commit_message>
Refactor Excel initialization and enhance medicine info processing
- Removed commented-out header row in Excel sheet initialization.
- Updated print statement in medicine info processing to include the medicine ID.
- Improved regex matching to extract and display additional medicine details.

This commit streamlines the Excel setup and enhances the output for better clarity during processing.
</commit_message>
<xml_diff>
--- a/中药信息.xlsx
+++ b/中药信息.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="中药信息" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,52 +414,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>药名</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>史载于</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>别名</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>性味归经</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>药材简介</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>用法用量</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>注意事项</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>